<commit_message>
reran with new weather data
</commit_message>
<xml_diff>
--- a/Lance/Result.xlsx
+++ b/Lance/Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nghia\Downloads\D95\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenglanfeng/Documents/GitHub/STAD95_W23/Lance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B45D7E-A120-4F05-801F-AE2515BDA551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2F55BD-9F10-E447-935D-D998D76EB82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13" yWindow="720" windowWidth="25587" windowHeight="15280" xr2:uid="{10646AE0-4AD5-9647-8521-C28DD3213C4A}"/>
+    <workbookView xWindow="-33020" yWindow="1360" windowWidth="33600" windowHeight="20500" xr2:uid="{10646AE0-4AD5-9647-8521-C28DD3213C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Model</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>Gaussian Process</t>
+  </si>
+  <si>
+    <t>SARIMA_2_xreg</t>
+  </si>
+  <si>
+    <t>Price_MAPE</t>
+  </si>
+  <si>
+    <t>Demand_MAPE</t>
   </si>
 </sst>
 </file>
@@ -461,20 +470,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83BBFC5-3D69-004A-8788-557BE20D268F}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,8 +500,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -508,7 +524,7 @@
         <v>1623311682</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -524,8 +540,14 @@
       <c r="E3" s="1">
         <v>414561058</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3">
+        <v>0.33993469999999998</v>
+      </c>
+      <c r="G3">
+        <v>4.0895910000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -541,8 +563,14 @@
       <c r="E4" s="1">
         <v>414561272</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>4.0895920000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -558,8 +586,14 @@
       <c r="E5">
         <v>326372945</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5">
+        <v>0.3273797</v>
+      </c>
+      <c r="G5">
+        <v>3.8295650000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -576,7 +610,7 @@
         <v>326427076</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -592,8 +626,14 @@
       <c r="E7">
         <v>328902644</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7">
+        <v>0.30023729999999998</v>
+      </c>
+      <c r="G7">
+        <v>3.8417069999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -609,8 +649,26 @@
       <c r="E8">
         <v>329027936</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F8">
+        <v>0.29989909999999997</v>
+      </c>
+      <c r="G8">
+        <v>3.8596079999999998E-2</v>
+      </c>
+      <c r="H8">
+        <v>12.63273</v>
+      </c>
+      <c r="I8">
+        <v>273.07889999999998</v>
+      </c>
+      <c r="J8">
+        <v>14438.61</v>
+      </c>
+      <c r="K8">
+        <v>330403616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -627,7 +685,7 @@
         <v>1839698615</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -644,7 +702,7 @@
         <v>1838608713</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -655,7 +713,7 @@
         <v>280.92280228024299</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -666,7 +724,7 @@
         <v>145.28645322483999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -677,7 +735,7 @@
         <v>59.054590527077899</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -688,7 +746,7 @@
         <v>768.21934369665905</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -699,7 +757,7 @@
         <v>109.99700622798299</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -710,7 +768,7 @@
         <v>1797760957.56164</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -721,7 +779,7 @@
         <v>811.20301807905798</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -730,6 +788,29 @@
       </c>
       <c r="C18">
         <v>274.90800754131197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19">
+        <v>0.32682860000000002</v>
+      </c>
+      <c r="G19">
+        <v>3.8431569999999998E-2</v>
+      </c>
+      <c r="H19">
+        <v>12.49192</v>
+      </c>
+      <c r="I19">
+        <v>268.31880000000001</v>
+      </c>
+      <c r="J19">
+        <v>14369.06</v>
+      </c>
+      <c r="K19">
+        <v>327475674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>